<commit_message>
modified template file and query as per requirement
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/assessment_report_template.xlsx
+++ b/webroot/export/customexcel/default_templates/assessment_report_template.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pocor-openemis-core\webroot\export\customexcel\default_templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D1B356-93FD-4312-A261-CD60EB40C1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="760" windowWidth="27320" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="4" r:id="rId1"/>
@@ -24,9 +30,6 @@
     <t>Grade:</t>
   </si>
   <si>
-    <t>${Assessments.education_grade.name}</t>
-  </si>
-  <si>
     <t>Class:</t>
   </si>
   <si>
@@ -67,13 +70,16 @@
   </si>
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"67","imageMarginLeft":"10","imageMarginTop":"1"}}</t>
+  </si>
+  <si>
+    <t>${EducationGrades.name}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -394,7 +400,7 @@
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -730,14 +736,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AG11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="2.83203125" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
@@ -756,23 +762,23 @@
     </row>
     <row r="2" spans="2:33" ht="25" customHeight="1">
       <c r="B2" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F2" s="14"/>
     </row>
     <row r="3" spans="2:33" ht="25" customHeight="1">
       <c r="B3" s="21"/>
       <c r="C3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>2</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>3</v>
       </c>
       <c r="F3" s="9"/>
     </row>
@@ -783,19 +789,19 @@
     </row>
     <row r="5" spans="2:33" s="1" customFormat="1" ht="40" customHeight="1">
       <c r="B5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>12</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AG5" s="6"/>
     </row>
@@ -813,25 +819,25 @@
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AG7" s="6"/>
     </row>
     <row r="8" spans="2:33" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="D8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>14</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:33">

</xml_diff>